<commit_message>
fit data to model
</commit_message>
<xml_diff>
--- a/corticalflow.xlsx
+++ b/corticalflow.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rainxiong/Desktop/Sugioka Lab/For Eric cortical flow/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcuslai/Desktop/Codes/Python/cell simulation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AF85B43-0093-584E-AA2E-2C01B3839DD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB901B59-2523-EA4A-B268-3F95FC164FC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="960" windowWidth="27640" windowHeight="15680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="760" yWindow="960" windowWidth="27640" windowHeight="15680" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Annotation" sheetId="2" r:id="rId1"/>
-    <sheet name="IntactKSG4-WT-corticalflow-umpe" sheetId="1" r:id="rId2"/>
+    <sheet name="corticalflow" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -1285,7 +1285,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A16:A21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
@@ -1326,7 +1326,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:U53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>

</xml_diff>